<commit_message>
Controle de Caixa + Notas Fiscais + Documentos dos funcionários
</commit_message>
<xml_diff>
--- a/2020/CONTROLE DE CAIXA DEZEMBRO 2020/07-12-2020_FluxoDeCaixa.xlsx
+++ b/2020/CONTROLE DE CAIXA DEZEMBRO 2020/07-12-2020_FluxoDeCaixa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adm\Documents\GitHub\ConnectFibra\2020\CONTROLE DE CAIXA DEZEMBRO 2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CD2830-CDF8-4AAF-ACDC-69E6469F9B6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C698F547-2831-454E-86E2-5DA1A4C61DF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Caixa de Amanda" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
   <si>
     <t>FLUXO CAIXA DIÁRIO</t>
   </si>
@@ -100,6 +100,21 @@
   </si>
   <si>
     <t>Gasolina Moto</t>
+  </si>
+  <si>
+    <t>Vale Paulista</t>
+  </si>
+  <si>
+    <t>Vale Luciano</t>
+  </si>
+  <si>
+    <t>Vale Jessica</t>
+  </si>
+  <si>
+    <t>Plug tomada de saída</t>
+  </si>
+  <si>
+    <t>Dupla Fase</t>
   </si>
 </sst>
 </file>
@@ -577,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +641,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="9">
-        <v>470</v>
+        <v>550</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -664,8 +679,8 @@
         <v>5</v>
       </c>
       <c r="B10" s="8">
-        <f>SUM(B15:B22)</f>
-        <v>517</v>
+        <f>SUM(B15:B25)</f>
+        <v>566.5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -680,7 +695,7 @@
       </c>
       <c r="B12" s="8">
         <f>(B6+B7+B4)-B10</f>
-        <v>-22.149999999999977</v>
+        <v>8.3500000000000227</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -760,19 +775,43 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="15"/>
+      <c r="A23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="15">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="15">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="15">
+        <v>24.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="15"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+      <c r="B27" s="4">
+        <v>8.35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -785,10 +824,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,7 +852,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="5">
-        <v>44171</v>
+        <v>44172</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -833,7 +872,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="9">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -864,7 +903,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="9">
-        <v>0</v>
+        <v>585.70000000000005</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -873,8 +912,8 @@
         <v>5</v>
       </c>
       <c r="B10" s="8">
-        <f>SUM(B15:B18)</f>
-        <v>0</v>
+        <f>SUM(B15:B16)</f>
+        <v>50</v>
       </c>
       <c r="D10" s="2"/>
     </row>
@@ -907,38 +946,38 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
+      <c r="A15" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="15">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
+      <c r="A16" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="15">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="18"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
+      <c r="A18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="21">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="18"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="21">
-        <v>0</v>
-      </c>
+      <c r="B19" s="15"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="15"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
+      <c r="B21" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1095,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,7 +1160,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="5">
-        <v>44171</v>
+        <v>44172</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1139,7 +1178,7 @@
       </c>
       <c r="B5" s="9">
         <f>SUM('Caixa de Jessica'!B6,'Caixa de Amanda'!B6)</f>
-        <v>470</v>
+        <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1173,7 +1212,7 @@
       </c>
       <c r="B8" s="6">
         <f>SUM('Caixa de Jessica'!B9,'Caixa de Rose'!B9,'Caixa de Amanda'!B9)</f>
-        <v>667.4</v>
+        <v>1253.0999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1182,7 +1221,7 @@
       </c>
       <c r="B9" s="8">
         <f>SUM('Caixa de Jessica'!B10,'Caixa de Rose'!B10,'Caixa de Amanda'!B10)</f>
-        <v>517</v>
+        <v>616.5</v>
       </c>
       <c r="F9" s="13"/>
     </row>
@@ -1196,7 +1235,7 @@
       </c>
       <c r="B11" s="11">
         <f>(B5+B6+B4)-B9</f>
-        <v>-22.149999999999977</v>
+        <v>8.3500000000000227</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1204,8 +1243,8 @@
         <v>9</v>
       </c>
       <c r="B13" s="22">
-        <f>SUM('Caixa de Jessica'!B20,'Caixa de Amanda'!B24)</f>
-        <v>0</v>
+        <f>SUM('Caixa de Jessica'!B18,'Caixa de Amanda'!B27)</f>
+        <v>8.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>